<commit_message>
Updates to workbooks over the last few days, made as I read over/reviewed old code
</commit_message>
<xml_diff>
--- a/results/2023-0215/notebook/GEO-submission-workbook_details.xlsx
+++ b/results/2023-0215/notebook/GEO-submission-workbook_details.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavatt/projects-etc/2022_transcriptome-construction/results/2023-0215/notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalavattam/Dropbox/FHCC/2022_transcriptome-construction/results/2023-0215/notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F7AF6FC-ACB9-7347-AEE6-FCD3CBBEAE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAA47D9-DDFB-D44D-B0CB-452EA70848CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7700" windowWidth="38400" windowHeight="21100" xr2:uid="{596A90F4-9442-3846-B7E1-FF5DD53DAC6B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{596A90F4-9442-3846-B7E1-FF5DD53DAC6B}"/>
   </bookViews>
   <sheets>
     <sheet name="organized file array" sheetId="1" r:id="rId1"/>
-    <sheet name="#TMP" sheetId="2" r:id="rId2"/>
+    <sheet name="supplementary files" sheetId="4" r:id="rId2"/>
+    <sheet name="#TMP" sheetId="2" r:id="rId3"/>
+    <sheet name="data processing steps" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -2227,8 +2229,478 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>NCBI User</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2DC2F850-EA93-EB4E-A592-0019155BB522}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Provide details of how processed data files were generated. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{F6215D03-A730-DF4F-A0C9-73EC0E77EDB9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Provide details of how processed data files were generated. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{A55F9745-79A9-0946-AA17-D367FB62B7DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Provide details of how processed data files were generated. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{2EF79F94-F234-4948-90E6-BF83DF31B24F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Provide details of how processed data files were generated. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{5907A1D5-D54D-DD48-A0BC-21F469F13C2F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Provide details of how processed data files were generated. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Steps may include:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base-calling software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Data filtering steps;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Read alignment software, version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">etc.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="374">
   <si>
     <t>Nab3-AID_Q_day7_tcn_N_auxT_tcF_7716_rep1_batch1.UTPD.bam</t>
   </si>
@@ -3335,13 +3807,72 @@
   </si>
   <si>
     <t>Greenlaw-et-al.txome_representative-pa-ncRNA.hc_strd-eq_nonuniq-none.tsv</t>
+  </si>
+  <si>
+    <t>*data processing step</t>
+  </si>
+  <si>
+    <t>Gene Transfer Format (gtf) and Gene Feature Format (gff3) files were obtained or derived from publicly available sources using custom scripts. Additionally, some files were generated via nascent transcriptome assembly and annotation using Trinity, GffRead, and custom scripts. To perform feature-level quantification, we used htseq-count with the gtf and gff3 files, and filtered, UMI-deduplicated, non-k-mer-adjusted bams. For more details, see Greenlaw, Alavattam, and Tsukiyama.</t>
+  </si>
+  <si>
+    <t>Paired-end reads underwent quality assessment with FastQC and MultiQC. Unique Molecular Identifier (UMI) sequences were appended to the reads using UMI-tools, and adapter and quality trimming were performed with Atria. For nascent transcriptome assembly, reads were additionally subjected to k-mer adjustment using Rcorrector. For more details, see Greenlaw, Alavattam, and Tsukiyama.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using the aligner STAR, processed reads were aligned to a concatenated multi-organism reference genome consisting of the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S. cerevisiae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K. lactis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and 20S narnavirus genomes. Non-k-mer-adjusted bams were indexed and filtered (with Samtools) to retain only primary alignments, while k-mer-adjusted bams were indexed and filtered to retain both primary and secondary alignments. After alignment filtering, technical duplicates were removed from the bams using UMI-tools. For more details, see Greenlaw, Alavattam, and Tsukiyama.</t>
+    </r>
+  </si>
+  <si>
+    <t>To generate normalized coverage tracks (*.bw), we used non-k-mer-adjusted bams as input to the utility bamCoverage (deepTools) in one of two ways: (a) For the bins per million (BPM) normalization method, mapped reads were normalized by their library size while excluding all rRNA and tRNA regions. The bin size for this method was set to 1 base pair. (b) For the scaled coverage (SC) method, library size estimates were first calculated using K. lactis spike-in counts. The bam files were then processed by supplying the reciprocals of the estimates as arguments (--scaleFactor) to bamCoverage. Again, the bin size was set to 1 base pair. For more details, see Greenlaw, Alavattam, and Tsukiyama.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3401,6 +3932,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -3447,7 +3993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3471,6 +4017,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -4150,10 +4705,10 @@
   <dimension ref="A1:AD45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7506,32 +8061,32 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:G21 E23:G29 E31:G45">
+    <cfRule type="duplicateValues" dxfId="35" priority="29"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H2:H17">
-    <cfRule type="duplicateValues" dxfId="35" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H23 I22">
-    <cfRule type="duplicateValues" dxfId="34" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:H45 I30">
-    <cfRule type="duplicateValues" dxfId="33" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:I41 I32:I35">
-    <cfRule type="duplicateValues" dxfId="32" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:Q2">
-    <cfRule type="duplicateValues" dxfId="31" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:Q9 J33:Q45 J32:K32 M32:Q32 J11:Q31 J10 L10:Q10">
-    <cfRule type="duplicateValues" dxfId="30" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="33"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA40:AA78">
-    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA23:AA39 AA21 AA2:AB17">
-    <cfRule type="duplicateValues" dxfId="28" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:G21 E23:G29 E31:G45">
-    <cfRule type="duplicateValues" dxfId="27" priority="29"/>
+  <conditionalFormatting sqref="L32">
+    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Z9">
     <cfRule type="duplicateValues" dxfId="26" priority="28"/>
@@ -7548,71 +8103,71 @@
   <conditionalFormatting sqref="Y32:Z37">
     <cfRule type="duplicateValues" dxfId="22" priority="54"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Y38:Z40">
+    <cfRule type="duplicateValues" dxfId="21" priority="23"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Y41:Z45">
-    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y38:Z40">
-    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
+  <conditionalFormatting sqref="AA23:AA39 AA21 AA2:AB17">
+    <cfRule type="duplicateValues" dxfId="19" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA40:AA78">
+    <cfRule type="duplicateValues" dxfId="18" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC3:AD3">
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC5:AD5">
+    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC7:AD7">
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8:AD8 AC6:AD6 AC4:AD4 AC2:AD2">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AD3">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC5:AD5">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC7:AD7">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC9:AD9">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC19:AD19">
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC21:AD21">
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC22:AD22 AC20:AD20 AC18:AD18">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC19:AD19">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC21:AD21">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC23:AD23">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC33:AD33">
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC35:AD35">
+    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC36:AD36 AC34:AD34 AC32:AD32">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC33:AD33">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC35:AD35">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC37:AD37">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC44:AD44 AC42:AD42 AC40:AD40 AC38:AD38">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC45:AD45">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC43:AD43">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="AC39:AD39">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC41:AD41">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC39:AD39">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="AC43:AD43">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L32">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="AC44:AD44 AC42:AD42 AC40:AD40 AC38:AD38">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="AC45:AD45">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="Identify the organism(s) from which the sequences were derived.  For example:_x000a_Homo sapiens_x000a_Mus musculus_x000a_Arabidopsis thaliana_x000a_Escherichia coli K-12_x000a_Caenorhabditis elegans" sqref="E30:G30" xr:uid="{0E2D13D5-B00F-BF4F-912F-D54672ABE9A7}"/>
@@ -7624,6 +8179,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5751F5-2A8E-9344-A2B2-F3C61EA945D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4CFD51-87D4-4C41-AC6D-57FABAA1A824}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7635,4 +8202,62 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998D7465-F540-3843-8350-F13A302EB55D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="180" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>